<commit_message>
docs: add documentation section and improve README.md
</commit_message>
<xml_diff>
--- a/src/output/excel/1.xlsx
+++ b/src/output/excel/1.xlsx
@@ -493,7 +493,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>27/08/2023</t>
+          <t>28/08/2023</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>27/08/2023</t>
+          <t>28/08/2023</t>
         </is>
       </c>
     </row>
@@ -557,7 +557,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>27/08/2023</t>
+          <t>28/08/2023</t>
         </is>
       </c>
     </row>
@@ -589,7 +589,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>28/08/2023</t>
+          <t>29/08/2023</t>
         </is>
       </c>
     </row>
@@ -621,7 +621,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>28/08/2023</t>
+          <t>29/08/2023</t>
         </is>
       </c>
     </row>
@@ -653,7 +653,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>28/08/2023</t>
+          <t>29/08/2023</t>
         </is>
       </c>
     </row>
@@ -685,7 +685,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>28/08/2023</t>
+          <t>29/08/2023</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>28/08/2023</t>
+          <t>29/08/2023</t>
         </is>
       </c>
     </row>
@@ -749,7 +749,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>27/08/2023</t>
+          <t>28/08/2023</t>
         </is>
       </c>
     </row>
@@ -781,7 +781,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>27/08/2023</t>
+          <t>28/08/2023</t>
         </is>
       </c>
     </row>
@@ -813,7 +813,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>27/08/2023</t>
+          <t>28/08/2023</t>
         </is>
       </c>
     </row>
@@ -845,7 +845,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>28/08/2023</t>
+          <t>29/08/2023</t>
         </is>
       </c>
     </row>
@@ -877,7 +877,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>28/08/2023</t>
+          <t>29/08/2023</t>
         </is>
       </c>
     </row>
@@ -909,7 +909,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>28/08/2023</t>
+          <t>29/08/2023</t>
         </is>
       </c>
     </row>
@@ -941,7 +941,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>28/08/2023</t>
+          <t>29/08/2023</t>
         </is>
       </c>
     </row>
@@ -973,7 +973,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>28/08/2023</t>
+          <t>29/08/2023</t>
         </is>
       </c>
     </row>
@@ -1005,7 +1005,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>27/08/2023</t>
+          <t>28/08/2023</t>
         </is>
       </c>
     </row>
@@ -1037,7 +1037,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>27/08/2023</t>
+          <t>28/08/2023</t>
         </is>
       </c>
     </row>
@@ -1069,7 +1069,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>27/08/2023</t>
+          <t>28/08/2023</t>
         </is>
       </c>
     </row>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>28/08/2023</t>
+          <t>29/08/2023</t>
         </is>
       </c>
     </row>
@@ -1133,7 +1133,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>28/08/2023</t>
+          <t>29/08/2023</t>
         </is>
       </c>
     </row>
@@ -1165,7 +1165,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>28/08/2023</t>
+          <t>29/08/2023</t>
         </is>
       </c>
     </row>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>28/08/2023</t>
+          <t>29/08/2023</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>28/08/2023</t>
+          <t>29/08/2023</t>
         </is>
       </c>
     </row>

</xml_diff>